<commit_message>
FC Align Initial commit
</commit_message>
<xml_diff>
--- a/Hardware/Pro/Requirements.xlsx
+++ b/Hardware/Pro/Requirements.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="37660" windowHeight="23560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-27420" yWindow="920" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="185">
   <si>
     <t>Pin</t>
   </si>
@@ -555,6 +555,27 @@
   </si>
   <si>
     <t>UART4 (OSD)</t>
+  </si>
+  <si>
+    <t>PackGPS</t>
+  </si>
+  <si>
+    <t>PackAttitude</t>
+  </si>
+  <si>
+    <t>PackBatteryPack</t>
+  </si>
+  <si>
+    <t>PackHeartbeat</t>
+  </si>
+  <si>
+    <t>PackRCOut</t>
+  </si>
+  <si>
+    <t>PackSystemStatus</t>
+  </si>
+  <si>
+    <t>PackVFRHud</t>
   </si>
 </sst>
 </file>
@@ -688,8 +709,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -798,7 +857,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="111">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -835,6 +894,25 @@
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -871,6 +949,25 @@
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1346,7 +1443,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2365,19 +2462,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>141</v>
       </c>
@@ -2391,7 +2489,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -2399,7 +2497,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -2419,7 +2517,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2436,7 +2534,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>146</v>
       </c>
@@ -2456,7 +2554,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -2476,7 +2574,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2493,7 +2591,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -2510,7 +2608,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -2524,7 +2622,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -2532,7 +2630,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>152</v>
       </c>
@@ -2540,7 +2638,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>153</v>
       </c>
@@ -2548,7 +2646,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -2558,9 +2656,121 @@
       <c r="C13" t="s">
         <v>175</v>
       </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>179</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>184</v>
+      </c>
+      <c r="L15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>182</v>
+      </c>
+      <c r="L16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="10:13">
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>179</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13">
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>180</v>
+      </c>
+      <c r="L18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="10:13">
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>181</v>
+      </c>
+      <c r="L19">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="10:13">
+      <c r="J20">
+        <v>7</v>
+      </c>
+      <c r="K20" t="s">
+        <v>182</v>
+      </c>
+      <c r="L20">
+        <v>400</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="10:13">
+      <c r="J21">
+        <v>8</v>
+      </c>
+      <c r="K21" t="s">
+        <v>179</v>
+      </c>
+      <c r="L21">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="22" spans="10:13">
+      <c r="J22">
+        <v>9</v>
+      </c>
+      <c r="K22" t="s">
+        <v>183</v>
+      </c>
+      <c r="L22">
+        <v>500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>